<commit_message>
Now gives Survey Numbers
</commit_message>
<xml_diff>
--- a/surveys/INIS-061620-1794.xlsx
+++ b/surveys/INIS-061620-1794.xlsx
@@ -2877,6 +2877,513 @@
     </indexedColors>
   </colors>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <twoCellAnchor editAs="oneCell">
+    <from>
+      <col>21</col>
+      <colOff>46464</colOff>
+      <row>0</row>
+      <rowOff>55756</rowOff>
+    </from>
+    <to>
+      <col>24</col>
+      <colOff>450696</colOff>
+      <row>2</row>
+      <rowOff>181313</rowOff>
+    </to>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="3" name="Picture 2"/>
+        <cNvPicPr>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
+        </cNvPicPr>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId1"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="10291647" y="55756"/>
+          <a:ext cx="1867829" cy="580898"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <avLst/>
+        </a:prstGeom>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </twoCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <twoCellAnchor editAs="oneCell">
+    <from>
+      <col>21</col>
+      <colOff>46464</colOff>
+      <row>0</row>
+      <rowOff>55756</rowOff>
+    </from>
+    <to>
+      <col>24</col>
+      <colOff>450696</colOff>
+      <row>2</row>
+      <rowOff>181313</rowOff>
+    </to>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="2" name="Picture 1"/>
+        <cNvPicPr>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
+        </cNvPicPr>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId1"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="10247739" y="55756"/>
+          <a:ext cx="1861557" cy="582757"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <avLst/>
+        </a:prstGeom>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </twoCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <twoCellAnchor editAs="oneCell">
+    <from>
+      <col>21</col>
+      <colOff>46464</colOff>
+      <row>0</row>
+      <rowOff>55756</rowOff>
+    </from>
+    <to>
+      <col>24</col>
+      <colOff>450696</colOff>
+      <row>2</row>
+      <rowOff>181313</rowOff>
+    </to>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="2" name="Picture 1"/>
+        <cNvPicPr>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
+        </cNvPicPr>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId1"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="10247739" y="55756"/>
+          <a:ext cx="1861557" cy="582757"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <avLst/>
+        </a:prstGeom>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </twoCellAnchor>
+  <twoCellAnchor editAs="oneCell">
+    <from>
+      <col>0</col>
+      <colOff>302557</colOff>
+      <row>1</row>
+      <rowOff>11206</rowOff>
+    </from>
+    <to>
+      <col>7</col>
+      <colOff>40498</colOff>
+      <row>11</row>
+      <rowOff>103214</rowOff>
+    </to>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="3" name="Picture 2"/>
+        <cNvPicPr>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
+        </cNvPicPr>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId2"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="302557" y="235324"/>
+          <a:ext cx="3110912" cy="2333184"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <avLst/>
+        </a:prstGeom>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </twoCellAnchor>
+  <twoCellAnchor editAs="oneCell">
+    <from>
+      <col>14</col>
+      <colOff>262059</colOff>
+      <row>1</row>
+      <rowOff>15530</rowOff>
+    </from>
+    <to>
+      <col>21</col>
+      <colOff>0</colOff>
+      <row>11</row>
+      <rowOff>107538</rowOff>
+    </to>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="4" name="Picture 3"/>
+        <cNvPicPr>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
+        </cNvPicPr>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId3"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="7008000" y="239648"/>
+          <a:ext cx="3110912" cy="2333184"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <avLst/>
+        </a:prstGeom>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </twoCellAnchor>
+  <twoCellAnchor editAs="oneCell">
+    <from>
+      <col>7</col>
+      <colOff>266380</colOff>
+      <row>1</row>
+      <rowOff>8648</rowOff>
+    </from>
+    <to>
+      <col>14</col>
+      <colOff>4322</colOff>
+      <row>11</row>
+      <rowOff>100656</rowOff>
+    </to>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="5" name="Picture 4"/>
+        <cNvPicPr>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
+        </cNvPicPr>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId4"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="3639351" y="232766"/>
+          <a:ext cx="3110912" cy="2333184"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <avLst/>
+        </a:prstGeom>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </twoCellAnchor>
+  <twoCellAnchor editAs="oneCell">
+    <from>
+      <col>19</col>
+      <colOff>293114</colOff>
+      <row>20</row>
+      <rowOff>113821</rowOff>
+    </from>
+    <to>
+      <col>24</col>
+      <colOff>217033</colOff>
+      <row>33</row>
+      <rowOff>19850</rowOff>
+    </to>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="6" name="Picture 5"/>
+        <cNvPicPr>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
+        </cNvPicPr>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId5"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="9448320" y="5021997"/>
+          <a:ext cx="2333184" cy="3110912"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <avLst/>
+        </a:prstGeom>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </twoCellAnchor>
+  <twoCellAnchor editAs="oneCell">
+    <from>
+      <col>0</col>
+      <colOff>308647</colOff>
+      <row>11</row>
+      <rowOff>162972</rowOff>
+    </from>
+    <to>
+      <col>7</col>
+      <colOff>46588</colOff>
+      <row>20</row>
+      <rowOff>53274</rowOff>
+    </to>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="7" name="Picture 6"/>
+        <cNvPicPr>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
+        </cNvPicPr>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId6"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="308647" y="2628266"/>
+          <a:ext cx="3110912" cy="2333184"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <avLst/>
+        </a:prstGeom>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </twoCellAnchor>
+  <twoCellAnchor editAs="oneCell">
+    <from>
+      <col>0</col>
+      <colOff>301765</colOff>
+      <row>20</row>
+      <rowOff>144887</rowOff>
+    </from>
+    <to>
+      <col>7</col>
+      <colOff>39706</colOff>
+      <row>30</row>
+      <rowOff>12776</rowOff>
+    </to>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="8" name="Picture 7"/>
+        <cNvPicPr>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
+        </cNvPicPr>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId7"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="301765" y="5053063"/>
+          <a:ext cx="3110912" cy="2333184"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <avLst/>
+        </a:prstGeom>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </twoCellAnchor>
+  <twoCellAnchor editAs="oneCell">
+    <from>
+      <col>7</col>
+      <colOff>261265</colOff>
+      <row>11</row>
+      <rowOff>160411</rowOff>
+    </from>
+    <to>
+      <col>13</col>
+      <colOff>481060</colOff>
+      <row>20</row>
+      <rowOff>50713</rowOff>
+    </to>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="9" name="Picture 8"/>
+        <cNvPicPr>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
+        </cNvPicPr>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId8"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="3634236" y="2625705"/>
+          <a:ext cx="3110912" cy="2333184"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <avLst/>
+        </a:prstGeom>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </twoCellAnchor>
+  <twoCellAnchor editAs="oneCell">
+    <from>
+      <col>14</col>
+      <colOff>265586</colOff>
+      <row>11</row>
+      <rowOff>164736</rowOff>
+    </from>
+    <to>
+      <col>21</col>
+      <colOff>3527</colOff>
+      <row>20</row>
+      <rowOff>55038</rowOff>
+    </to>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="10" name="Picture 9"/>
+        <cNvPicPr>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
+        </cNvPicPr>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId9"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="7011527" y="2630030"/>
+          <a:ext cx="3110912" cy="2333184"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <avLst/>
+        </a:prstGeom>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </twoCellAnchor>
+  <twoCellAnchor editAs="oneCell">
+    <from>
+      <col>7</col>
+      <colOff>269911</colOff>
+      <row>20</row>
+      <rowOff>146648</rowOff>
+    </from>
+    <to>
+      <col>14</col>
+      <colOff>7853</colOff>
+      <row>30</row>
+      <rowOff>14537</rowOff>
+    </to>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="11" name="Picture 10"/>
+        <cNvPicPr>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
+        </cNvPicPr>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId10"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="3642882" y="5054824"/>
+          <a:ext cx="3110912" cy="2333184"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <avLst/>
+        </a:prstGeom>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </twoCellAnchor>
+</wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3611,7 +4118,7 @@
       <c r="O10" s="314" t="n"/>
       <c r="P10" s="345" t="n"/>
       <c r="Q10" s="227" t="n">
-        <v>0.74</v>
+        <v>0.3602</v>
       </c>
       <c r="R10" s="314" t="n"/>
       <c r="S10" s="314" t="n"/>
@@ -5738,6 +6245,7 @@
     <firstHeader/>
     <firstFooter/>
   </headerFooter>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -6212,7 +6720,7 @@
       <c r="O10" s="314" t="n"/>
       <c r="P10" s="345" t="n"/>
       <c r="Q10" s="227" t="n">
-        <v>0.74</v>
+        <v>0.3602</v>
       </c>
       <c r="R10" s="314" t="n"/>
       <c r="S10" s="314" t="n"/>
@@ -8159,6 +8667,7 @@
     <firstHeader/>
     <firstFooter/>
   </headerFooter>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -9323,5 +9832,6 @@
     <firstHeader/>
     <firstFooter/>
   </headerFooter>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>